<commit_message>
More code on vstring
</commit_message>
<xml_diff>
--- a/Learning/l19_vstring/vstring.xlsx
+++ b/Learning/l19_vstring/vstring.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Rust\Learning\l19_string\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Rust\Learning\l19_vstring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7944C833-5F76-4BA1-AB64-728F8E51F9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F7C516-9D31-46FC-93F7-AADF39552468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28035" yWindow="6540" windowWidth="23475" windowHeight="24990" xr2:uid="{749E69D6-895E-461B-A1ED-6BE4791DCD44}"/>
+    <workbookView xWindow="28230" yWindow="1095" windowWidth="23475" windowHeight="24990" xr2:uid="{749E69D6-895E-461B-A1ED-6BE4791DCD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t> u8</t>
   </si>
@@ -95,9 +95,6 @@
     <t>byteoption</t>
   </si>
   <si>
-    <t>bytevec</t>
-  </si>
-  <si>
     <t>byteiterator</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>glyphoption</t>
   </si>
   <si>
-    <t>charvec</t>
-  </si>
-  <si>
     <t>glyphvec</t>
   </si>
   <si>
@@ -165,6 +159,30 @@
   </si>
   <si>
     <t>Option&lt;&amp;str&gt;</t>
+  </si>
+  <si>
+    <t>get_glyph_from_byteindex</t>
+  </si>
+  <si>
+    <t>get_glyphoption_from_byteindex</t>
+  </si>
+  <si>
+    <t>get_byteslice_from_byteindex</t>
+  </si>
+  <si>
+    <t>bytevector</t>
+  </si>
+  <si>
+    <t>charvector</t>
+  </si>
+  <si>
+    <t>get_bytevector_from_byteindex</t>
+  </si>
+  <si>
+    <t>get_charvector_from_byteindex</t>
+  </si>
+  <si>
+    <t>get_glyphvector_from_byteindex</t>
   </si>
 </sst>
 </file>
@@ -539,14 +557,14 @@
   <dimension ref="A2:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -562,27 +580,27 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -593,7 +611,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -604,7 +622,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -615,7 +633,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -623,10 +641,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -634,7 +652,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -642,7 +663,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -650,7 +674,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -658,7 +685,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -666,7 +696,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -674,7 +707,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -682,7 +718,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -690,7 +726,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -698,7 +734,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -706,12 +742,12 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -719,7 +755,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started charrange and its tests
</commit_message>
<xml_diff>
--- a/Learning/l19_vstring/vstring.xlsx
+++ b/Learning/l19_vstring/vstring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Rust\Learning\l19_vstring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6F2056-677F-476A-BEFB-FFFB20BFA67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D516E2-0F6E-4A19-9E93-EC0AF1B070C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30540" yWindow="3900" windowWidth="23475" windowHeight="24990" xr2:uid="{749E69D6-895E-461B-A1ED-6BE4791DCD44}"/>
+    <workbookView xWindow="31215" yWindow="3840" windowWidth="23475" windowHeight="24990" xr2:uid="{749E69D6-895E-461B-A1ED-6BE4791DCD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
   <si>
     <t> u8</t>
   </si>
@@ -266,6 +266,11 @@
   </si>
   <si>
     <t>get_string_from_charindex</t>
+  </si>
+  <si>
+    <t>get_byteslice_from_charrange
+get_byteslice_from_startcharcount
+get_byteslice_from_endcharcount</t>
   </si>
 </sst>
 </file>
@@ -646,7 +651,7 @@
   <dimension ref="A2:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +661,7 @@
     <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.42578125" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -819,7 +824,9 @@
       <c r="E10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>

</xml_diff>

<commit_message>
charrange code done and tests ok
</commit_message>
<xml_diff>
--- a/Learning/l19_vstring/vstring.xlsx
+++ b/Learning/l19_vstring/vstring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Rust\Learning\l19_vstring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D516E2-0F6E-4A19-9E93-EC0AF1B070C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539D7F69-A178-4163-9886-F52BD89B109E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31215" yWindow="3840" windowWidth="23475" windowHeight="24990" xr2:uid="{749E69D6-895E-461B-A1ED-6BE4791DCD44}"/>
+    <workbookView xWindow="13365" yWindow="3570" windowWidth="23475" windowHeight="24990" xr2:uid="{749E69D6-895E-461B-A1ED-6BE4791DCD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
   <si>
     <t> u8</t>
   </si>
@@ -271,6 +271,30 @@
     <t>get_byteslice_from_charrange
 get_byteslice_from_startcharcount
 get_byteslice_from_endcharcount</t>
+  </si>
+  <si>
+    <t>get_bytevector_from_charrange</t>
+  </si>
+  <si>
+    <t>get_charvector_from_charrange</t>
+  </si>
+  <si>
+    <t>get_glyphvector_from_charrange</t>
+  </si>
+  <si>
+    <t>get_byteiterator_from_charrange</t>
+  </si>
+  <si>
+    <t>get_chariterator_from_charrange</t>
+  </si>
+  <si>
+    <t>get_glyphiterator_from_charrange</t>
+  </si>
+  <si>
+    <t>get_strref_from_charrange</t>
+  </si>
+  <si>
+    <t>get_string_from_charrange</t>
   </si>
 </sst>
 </file>
@@ -651,7 +675,7 @@
   <dimension ref="A2:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +870,9 @@
       <c r="E11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
@@ -866,7 +892,9 @@
       <c r="E12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
@@ -886,7 +914,9 @@
       <c r="E13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
@@ -906,7 +936,9 @@
       <c r="E14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
@@ -926,7 +958,9 @@
       <c r="E15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
@@ -946,7 +980,9 @@
       <c r="E16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
@@ -966,7 +1002,9 @@
       <c r="E17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
@@ -986,7 +1024,9 @@
       <c r="E18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>

</xml_diff>

<commit_message>
Started glyphindex and tests
</commit_message>
<xml_diff>
--- a/Learning/l19_vstring/vstring.xlsx
+++ b/Learning/l19_vstring/vstring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Rust\Learning\l19_vstring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539D7F69-A178-4163-9886-F52BD89B109E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E28D009-9A61-44A1-B0C9-068B273DD2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13365" yWindow="3570" windowWidth="23475" windowHeight="24990" xr2:uid="{749E69D6-895E-461B-A1ED-6BE4791DCD44}"/>
+    <workbookView xWindow="28215" yWindow="2970" windowWidth="23475" windowHeight="24990" xr2:uid="{749E69D6-895E-461B-A1ED-6BE4791DCD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t> u8</t>
   </si>
@@ -295,6 +295,39 @@
   </si>
   <si>
     <t>get_string_from_charrange</t>
+  </si>
+  <si>
+    <t>get_glyph_from_glyphindex</t>
+  </si>
+  <si>
+    <t>get_glyphoption_from_glyphindex</t>
+  </si>
+  <si>
+    <t>get_byteslice_from_glyphindex</t>
+  </si>
+  <si>
+    <t>get_bytevector_from_glyphindex</t>
+  </si>
+  <si>
+    <t>get_charvector_from_glyphindex</t>
+  </si>
+  <si>
+    <t>get_glyphvector_from_glyphindex</t>
+  </si>
+  <si>
+    <t>get_byteiterator_from_glyphindex</t>
+  </si>
+  <si>
+    <t>get_chariterator_from_glyphindex</t>
+  </si>
+  <si>
+    <t>get_glyphiterator_from_glyphindex</t>
+  </si>
+  <si>
+    <t>get_strref_from_glyphindex</t>
+  </si>
+  <si>
+    <t>get_string_from_glyphindex</t>
   </si>
 </sst>
 </file>
@@ -675,7 +708,7 @@
   <dimension ref="A2:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,10 +716,10 @@
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -811,7 +844,9 @@
         <v>64</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -829,7 +864,9 @@
         <v>65</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -851,7 +888,9 @@
       <c r="F10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -873,7 +912,9 @@
       <c r="F11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -895,7 +936,9 @@
       <c r="F12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -917,7 +960,9 @@
       <c r="F13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -939,7 +984,9 @@
       <c r="F14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -961,7 +1008,9 @@
       <c r="F15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -983,7 +1032,9 @@
       <c r="F16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1005,7 +1056,9 @@
       <c r="F17" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1027,7 +1080,9 @@
       <c r="F18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added get_string_from_charslice; toml 2021
</commit_message>
<xml_diff>
--- a/Learning/l19_vstring/vstring.xlsx
+++ b/Learning/l19_vstring/vstring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\Rust\Learning\l19_vstring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E450AB58-36EA-4515-8A6C-D811B062E074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B40FE9-7872-4CDA-A48B-CB431BB59D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="1830" windowWidth="36825" windowHeight="24990" xr2:uid="{749E69D6-895E-461B-A1ED-6BE4791DCD44}"/>
+    <workbookView xWindow="7170" yWindow="2400" windowWidth="24195" windowHeight="24990" xr2:uid="{749E69D6-895E-461B-A1ED-6BE4791DCD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
-  <si>
-    <t> u8</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="118">
   <si>
     <t>Option&lt;u8&gt;</t>
   </si>
@@ -358,13 +355,66 @@
 get_byteslice_from_startglyphcount
 get_byteslice_from_endglyphcount</t>
   </si>
+  <si>
+    <t>Conversions to String</t>
+  </si>
+  <si>
+    <t>String::from(str::from_utf8(byteslice).unwrap())</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>&amp;Vec&lt;u8&gt;</t>
+  </si>
+  <si>
+    <t>String::from_utf8(bytevector).unwrap()</t>
+  </si>
+  <si>
+    <t>String::from_utf8(byteiterator.collect::&lt;Vec&lt;u8&gt;&gt;()).unwrap()</t>
+  </si>
+  <si>
+    <t>String::from_iter(charvector)</t>
+  </si>
+  <si>
+    <t>&amp;Vec&lt;char&gt;</t>
+  </si>
+  <si>
+    <t>String::from_iter(chariterator)</t>
+  </si>
+  <si>
+    <t>String::from_iter(charvectorref)</t>
+  </si>
+  <si>
+    <t>String::from(str::from_utf8(bytevectorref).unwrap())</t>
+  </si>
+  <si>
+    <t>(and .to_string() variants)</t>
+  </si>
+  <si>
+    <t>u8</t>
+  </si>
+  <si>
+    <t>&amp;[char]</t>
+  </si>
+  <si>
+    <t>String::from_iter(charslice)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -392,13 +442,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDF6E9E-38C1-496D-A7A4-539D6BC9175C}">
-  <dimension ref="A2:H19"/>
+  <dimension ref="A2:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,52 +807,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -807,14 +861,14 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -823,313 +877,313 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
+      <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
+      <c r="A7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="H10" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1142,6 +1196,83 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>